<commit_message>
AH Up in 20200921
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="61">
   <si>
     <t>SearchString</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -242,13 +242,20 @@
   </si>
   <si>
     <t>关键字1校验</t>
+  </si>
+  <si>
+    <t>Allen_百度搜索</t>
+  </si>
+  <si>
+    <t>显示为 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,12 +770,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.75" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.75" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.75" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -800,6 +807,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -931,11 +941,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.75" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.75" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -972,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>19</v>
@@ -1104,13 +1114,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
-    <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="5" width="12.75" customWidth="1"/>
-    <col min="6" max="6" width="10.375" customWidth="1"/>
-    <col min="7" max="7" width="29.875" customWidth="1"/>
-    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.25" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.75" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1183,7 +1193,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="19.25" customWidth="1"/>
+    <col min="2" max="3" customWidth="true" width="19.25" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>